<commit_message>
Add CGV 25000100 at 20250224143500
</commit_message>
<xml_diff>
--- a/CGV/data/20250224143500/25000100/25000100.xlsx
+++ b/CGV/data/20250224143500/25000100/25000100.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3335" uniqueCount="2335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3335" uniqueCount="2334">
   <si>
     <t>Show</t>
   </si>
@@ -8065,9 +8065,6 @@
   </si>
   <si>
     <t>Province</t>
-  </si>
-  <si>
-    <t>Revenue2</t>
   </si>
 </sst>
 </file>
@@ -8164,7 +8161,7 @@
     <tableColumn id="5" name="Revenue" dataDxfId="1">
       <calculatedColumnFormula>SUMIF($C$7:$C$89,$H91,F$7:F$89)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Revenue2" dataDxfId="0">
+    <tableColumn id="6" name="Rate" dataDxfId="0">
       <calculatedColumnFormula>J91/(K91+J91)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8437,8 +8434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10182,7 +10179,7 @@
         <v>4</v>
       </c>
       <c r="M90" t="s">
-        <v>2334</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.25">
@@ -10190,23 +10187,23 @@
         <v>2301</v>
       </c>
       <c r="I91" s="1">
-        <f>COUNTIF($C$7:$C$89,$H91)</f>
+        <f t="shared" ref="I91:I122" si="0">COUNTIF($C$7:$C$89,$H91)</f>
         <v>21</v>
       </c>
       <c r="J91" s="1">
-        <f>SUMIF($C$7:$C$89,$H91,D$7:D$89)</f>
+        <f t="shared" ref="J91:J122" si="1">SUMIF($C$7:$C$89,$H91,D$7:D$89)</f>
         <v>12439</v>
       </c>
       <c r="K91" s="1">
-        <f>SUMIF($C$7:$C$89,$H91,E$7:E$89)</f>
+        <f t="shared" ref="K91:K122" si="2">SUMIF($C$7:$C$89,$H91,E$7:E$89)</f>
         <v>44926</v>
       </c>
       <c r="L91" s="1">
-        <f>SUMIF($C$7:$C$89,$H91,F$7:F$89)</f>
+        <f t="shared" ref="L91:L122" si="3">SUMIF($C$7:$C$89,$H91,F$7:F$89)</f>
         <v>2860970000</v>
       </c>
       <c r="M91" s="3">
-        <f>J91/(K91+J91)*100</f>
+        <f t="shared" ref="M91:M122" si="4">J91/(K91+J91)*100</f>
         <v>21.683953630262355</v>
       </c>
     </row>
@@ -10215,23 +10212,23 @@
         <v>2302</v>
       </c>
       <c r="I92" s="1">
-        <f>COUNTIF($C$7:$C$89,$H92)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="J92" s="1">
-        <f>SUMIF($C$7:$C$89,$H92,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>11792</v>
       </c>
       <c r="K92" s="1">
-        <f>SUMIF($C$7:$C$89,$H92,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>33939</v>
       </c>
       <c r="L92" s="1">
-        <f>SUMIF($C$7:$C$89,$H92,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>2712160000</v>
       </c>
       <c r="M92" s="3">
-        <f>J92/(K92+J92)*100</f>
+        <f t="shared" si="4"/>
         <v>25.785572150182588</v>
       </c>
     </row>
@@ -10240,23 +10237,23 @@
         <v>2306</v>
       </c>
       <c r="I93" s="1">
-        <f>COUNTIF($C$7:$C$89,$H93)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J93" s="1">
-        <f>SUMIF($C$7:$C$89,$H93,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>1025</v>
       </c>
       <c r="K93" s="1">
-        <f>SUMIF($C$7:$C$89,$H93,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>2274</v>
       </c>
       <c r="L93" s="1">
-        <f>SUMIF($C$7:$C$89,$H93,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>235750000</v>
       </c>
       <c r="M93" s="3">
-        <f>J93/(K93+J93)*100</f>
+        <f t="shared" si="4"/>
         <v>31.070021218551076</v>
       </c>
     </row>
@@ -10265,23 +10262,23 @@
         <v>2303</v>
       </c>
       <c r="I94" s="1">
-        <f>COUNTIF($C$7:$C$89,$H94)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J94" s="1">
-        <f>SUMIF($C$7:$C$89,$H94,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>977</v>
       </c>
       <c r="K94" s="1">
-        <f>SUMIF($C$7:$C$89,$H94,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>9271</v>
       </c>
       <c r="L94" s="1">
-        <f>SUMIF($C$7:$C$89,$H94,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>224710000</v>
       </c>
       <c r="M94" s="3">
-        <f>J94/(K94+J94)*100</f>
+        <f t="shared" si="4"/>
         <v>9.5335675253708043</v>
       </c>
     </row>
@@ -10290,23 +10287,23 @@
         <v>2304</v>
       </c>
       <c r="I95" s="1">
-        <f>COUNTIF($C$7:$C$89,$H95)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J95" s="1">
-        <f>SUMIF($C$7:$C$89,$H95,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>674</v>
       </c>
       <c r="K95" s="1">
-        <f>SUMIF($C$7:$C$89,$H95,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>4762</v>
       </c>
       <c r="L95" s="1">
-        <f>SUMIF($C$7:$C$89,$H95,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>155020000</v>
       </c>
       <c r="M95" s="3">
-        <f>J95/(K95+J95)*100</f>
+        <f t="shared" si="4"/>
         <v>12.398822663723326</v>
       </c>
     </row>
@@ -10315,23 +10312,23 @@
         <v>2310</v>
       </c>
       <c r="I96" s="1">
-        <f>COUNTIF($C$7:$C$89,$H96)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J96" s="1">
-        <f>SUMIF($C$7:$C$89,$H96,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>404</v>
       </c>
       <c r="K96" s="1">
-        <f>SUMIF($C$7:$C$89,$H96,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>3751</v>
       </c>
       <c r="L96" s="1">
-        <f>SUMIF($C$7:$C$89,$H96,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>92920000</v>
       </c>
       <c r="M96" s="3">
-        <f>J96/(K96+J96)*100</f>
+        <f t="shared" si="4"/>
         <v>9.7232250300842349</v>
       </c>
     </row>
@@ -10340,23 +10337,23 @@
         <v>2305</v>
       </c>
       <c r="I97" s="1">
-        <f>COUNTIF($C$7:$C$89,$H97)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J97" s="1">
-        <f>SUMIF($C$7:$C$89,$H97,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>321</v>
       </c>
       <c r="K97" s="1">
-        <f>SUMIF($C$7:$C$89,$H97,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1521</v>
       </c>
       <c r="L97" s="1">
-        <f>SUMIF($C$7:$C$89,$H97,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>73830000</v>
       </c>
       <c r="M97" s="3">
-        <f>J97/(K97+J97)*100</f>
+        <f t="shared" si="4"/>
         <v>17.426710097719869</v>
       </c>
     </row>
@@ -10365,23 +10362,23 @@
         <v>2307</v>
       </c>
       <c r="I98" s="1">
-        <f>COUNTIF($C$7:$C$89,$H98)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J98" s="1">
-        <f>SUMIF($C$7:$C$89,$H98,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>274</v>
       </c>
       <c r="K98" s="1">
-        <f>SUMIF($C$7:$C$89,$H98,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1986</v>
       </c>
       <c r="L98" s="1">
-        <f>SUMIF($C$7:$C$89,$H98,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>63020000</v>
       </c>
       <c r="M98" s="3">
-        <f>J98/(K98+J98)*100</f>
+        <f t="shared" si="4"/>
         <v>12.123893805309734</v>
       </c>
     </row>
@@ -10390,23 +10387,23 @@
         <v>2322</v>
       </c>
       <c r="I99" s="1">
-        <f>COUNTIF($C$7:$C$89,$H99)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J99" s="1">
-        <f>SUMIF($C$7:$C$89,$H99,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>254</v>
       </c>
       <c r="K99" s="1">
-        <f>SUMIF($C$7:$C$89,$H99,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1321</v>
       </c>
       <c r="L99" s="1">
-        <f>SUMIF($C$7:$C$89,$H99,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>58420000</v>
       </c>
       <c r="M99" s="3">
-        <f>J99/(K99+J99)*100</f>
+        <f t="shared" si="4"/>
         <v>16.126984126984127</v>
       </c>
     </row>
@@ -10415,23 +10412,23 @@
         <v>2330</v>
       </c>
       <c r="I100" s="1">
-        <f>COUNTIF($C$7:$C$89,$H100)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J100" s="1">
-        <f>SUMIF($C$7:$C$89,$H100,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>209</v>
       </c>
       <c r="K100" s="1">
-        <f>SUMIF($C$7:$C$89,$H100,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="L100" s="1">
-        <f>SUMIF($C$7:$C$89,$H100,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>48070000</v>
       </c>
       <c r="M100" s="3">
-        <f>J100/(K100+J100)*100</f>
+        <f t="shared" si="4"/>
         <v>66.139240506329116</v>
       </c>
     </row>
@@ -10440,23 +10437,23 @@
         <v>2319</v>
       </c>
       <c r="I101" s="1">
-        <f>COUNTIF($C$7:$C$89,$H101)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J101" s="1">
-        <f>SUMIF($C$7:$C$89,$H101,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="K101" s="1">
-        <f>SUMIF($C$7:$C$89,$H101,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>355</v>
       </c>
       <c r="L101" s="1">
-        <f>SUMIF($C$7:$C$89,$H101,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>36800000</v>
       </c>
       <c r="M101" s="3">
-        <f>J101/(K101+J101)*100</f>
+        <f t="shared" si="4"/>
         <v>31.067961165048541</v>
       </c>
     </row>
@@ -10465,23 +10462,23 @@
         <v>2331</v>
       </c>
       <c r="I102" s="1">
-        <f>COUNTIF($C$7:$C$89,$H102)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J102" s="1">
-        <f>SUMIF($C$7:$C$89,$H102,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
       <c r="K102" s="1">
-        <f>SUMIF($C$7:$C$89,$H102,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1172</v>
       </c>
       <c r="L102" s="1">
-        <f>SUMIF($C$7:$C$89,$H102,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>33120000</v>
       </c>
       <c r="M102" s="3">
-        <f>J102/(K102+J102)*100</f>
+        <f t="shared" si="4"/>
         <v>10.94224924012158</v>
       </c>
     </row>
@@ -10490,23 +10487,23 @@
         <v>2308</v>
       </c>
       <c r="I103" s="1">
-        <f>COUNTIF($C$7:$C$89,$H103)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J103" s="1">
-        <f>SUMIF($C$7:$C$89,$H103,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="K103" s="1">
-        <f>SUMIF($C$7:$C$89,$H103,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1625</v>
       </c>
       <c r="L103" s="1">
-        <f>SUMIF($C$7:$C$89,$H103,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>31280000</v>
       </c>
       <c r="M103" s="3">
-        <f>J103/(K103+J103)*100</f>
+        <f t="shared" si="4"/>
         <v>7.7228847245883028</v>
       </c>
     </row>
@@ -10515,23 +10512,23 @@
         <v>2329</v>
       </c>
       <c r="I104" s="1">
-        <f>COUNTIF($C$7:$C$89,$H104)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J104" s="1">
-        <f>SUMIF($C$7:$C$89,$H104,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
       <c r="K104" s="1">
-        <f>SUMIF($C$7:$C$89,$H104,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>734</v>
       </c>
       <c r="L104" s="1">
-        <f>SUMIF($C$7:$C$89,$H104,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>29670000</v>
       </c>
       <c r="M104" s="3">
-        <f>J104/(K104+J104)*100</f>
+        <f t="shared" si="4"/>
         <v>14.947856315179605</v>
       </c>
     </row>
@@ -10540,23 +10537,23 @@
         <v>2309</v>
       </c>
       <c r="I105" s="1">
-        <f>COUNTIF($C$7:$C$89,$H105)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J105" s="1">
-        <f>SUMIF($C$7:$C$89,$H105,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="K105" s="1">
-        <f>SUMIF($C$7:$C$89,$H105,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>830</v>
       </c>
       <c r="L105" s="1">
-        <f>SUMIF($C$7:$C$89,$H105,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>29440000</v>
       </c>
       <c r="M105" s="3">
-        <f>J105/(K105+J105)*100</f>
+        <f t="shared" si="4"/>
         <v>13.361169102296449</v>
       </c>
     </row>
@@ -10565,23 +10562,23 @@
         <v>2311</v>
       </c>
       <c r="I106" s="1">
-        <f>COUNTIF($C$7:$C$89,$H106)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J106" s="1">
-        <f>SUMIF($C$7:$C$89,$H106,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>121</v>
       </c>
       <c r="K106" s="1">
-        <f>SUMIF($C$7:$C$89,$H106,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>523</v>
       </c>
       <c r="L106" s="1">
-        <f>SUMIF($C$7:$C$89,$H106,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>27830000</v>
       </c>
       <c r="M106" s="3">
-        <f>J106/(K106+J106)*100</f>
+        <f t="shared" si="4"/>
         <v>18.788819875776397</v>
       </c>
     </row>
@@ -10590,23 +10587,23 @@
         <v>2314</v>
       </c>
       <c r="I107" s="1">
-        <f>COUNTIF($C$7:$C$89,$H107)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J107" s="1">
-        <f>SUMIF($C$7:$C$89,$H107,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="K107" s="1">
-        <f>SUMIF($C$7:$C$89,$H107,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="L107" s="1">
-        <f>SUMIF($C$7:$C$89,$H107,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>21850000</v>
       </c>
       <c r="M107" s="3">
-        <f>J107/(K107+J107)*100</f>
+        <f t="shared" si="4"/>
         <v>17.148014440433212</v>
       </c>
     </row>
@@ -10615,23 +10612,23 @@
         <v>2314</v>
       </c>
       <c r="I108" s="1">
-        <f>COUNTIF($C$7:$C$89,$H108)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J108" s="1">
-        <f>SUMIF($C$7:$C$89,$H108,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="K108" s="1">
-        <f>SUMIF($C$7:$C$89,$H108,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="L108" s="1">
-        <f>SUMIF($C$7:$C$89,$H108,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>21850000</v>
       </c>
       <c r="M108" s="3">
-        <f>J108/(K108+J108)*100</f>
+        <f t="shared" si="4"/>
         <v>17.148014440433212</v>
       </c>
     </row>
@@ -10640,23 +10637,23 @@
         <v>2315</v>
       </c>
       <c r="I109" s="1">
-        <f>COUNTIF($C$7:$C$89,$H109)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J109" s="1">
-        <f>SUMIF($C$7:$C$89,$H109,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="K109" s="1">
-        <f>SUMIF($C$7:$C$89,$H109,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1279</v>
       </c>
       <c r="L109" s="1">
-        <f>SUMIF($C$7:$C$89,$H109,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>21850000</v>
       </c>
       <c r="M109" s="3">
-        <f>J109/(K109+J109)*100</f>
+        <f t="shared" si="4"/>
         <v>6.9141193595342072</v>
       </c>
     </row>
@@ -10665,23 +10662,23 @@
         <v>2324</v>
       </c>
       <c r="I110" s="1">
-        <f>COUNTIF($C$7:$C$89,$H110)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J110" s="1">
-        <f>SUMIF($C$7:$C$89,$H110,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="K110" s="1">
-        <f>SUMIF($C$7:$C$89,$H110,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="L110" s="1">
-        <f>SUMIF($C$7:$C$89,$H110,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>20240000</v>
       </c>
       <c r="M110" s="3">
-        <f>J110/(K110+J110)*100</f>
+        <f t="shared" si="4"/>
         <v>7.9207920792079207</v>
       </c>
     </row>
@@ -10690,23 +10687,23 @@
         <v>2326</v>
       </c>
       <c r="I111" s="1">
-        <f>COUNTIF($C$7:$C$89,$H111)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J111" s="1">
-        <f>SUMIF($C$7:$C$89,$H111,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="K111" s="1">
-        <f>SUMIF($C$7:$C$89,$H111,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1039</v>
       </c>
       <c r="L111" s="1">
-        <f>SUMIF($C$7:$C$89,$H111,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>19780000</v>
       </c>
       <c r="M111" s="3">
-        <f>J111/(K111+J111)*100</f>
+        <f t="shared" si="4"/>
         <v>7.6444444444444439</v>
       </c>
     </row>
@@ -10715,23 +10712,23 @@
         <v>2325</v>
       </c>
       <c r="I112" s="1">
-        <f>COUNTIF($C$7:$C$89,$H112)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J112" s="1">
-        <f>SUMIF($C$7:$C$89,$H112,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="K112" s="1">
-        <f>SUMIF($C$7:$C$89,$H112,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>736</v>
       </c>
       <c r="L112" s="1">
-        <f>SUMIF($C$7:$C$89,$H112,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>19090000</v>
       </c>
       <c r="M112" s="3">
-        <f>J112/(K112+J112)*100</f>
+        <f t="shared" si="4"/>
         <v>10.134310134310134</v>
       </c>
     </row>
@@ -10740,23 +10737,23 @@
         <v>2317</v>
       </c>
       <c r="I113" s="1">
-        <f>COUNTIF($C$7:$C$89,$H113)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J113" s="1">
-        <f>SUMIF($C$7:$C$89,$H113,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="K113" s="1">
-        <f>SUMIF($C$7:$C$89,$H113,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1437</v>
       </c>
       <c r="L113" s="1">
-        <f>SUMIF($C$7:$C$89,$H113,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>12650000</v>
       </c>
       <c r="M113" s="3">
-        <f>J113/(K113+J113)*100</f>
+        <f t="shared" si="4"/>
         <v>3.6863270777479888</v>
       </c>
     </row>
@@ -10765,23 +10762,23 @@
         <v>2318</v>
       </c>
       <c r="I114" s="1">
-        <f>COUNTIF($C$7:$C$89,$H114)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J114" s="1">
-        <f>SUMIF($C$7:$C$89,$H114,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="K114" s="1">
-        <f>SUMIF($C$7:$C$89,$H114,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>810</v>
       </c>
       <c r="L114" s="1">
-        <f>SUMIF($C$7:$C$89,$H114,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>8510000</v>
       </c>
       <c r="M114" s="3">
-        <f>J114/(K114+J114)*100</f>
+        <f t="shared" si="4"/>
         <v>4.3683589138134593</v>
       </c>
     </row>
@@ -10790,23 +10787,23 @@
         <v>2312</v>
       </c>
       <c r="I115" s="1">
-        <f>COUNTIF($C$7:$C$89,$H115)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J115" s="1">
-        <f>SUMIF($C$7:$C$89,$H115,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="K115" s="1">
-        <f>SUMIF($C$7:$C$89,$H115,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>619</v>
       </c>
       <c r="L115" s="1">
-        <f>SUMIF($C$7:$C$89,$H115,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>8280000</v>
       </c>
       <c r="M115" s="3">
-        <f>J115/(K115+J115)*100</f>
+        <f t="shared" si="4"/>
         <v>5.4961832061068705</v>
       </c>
     </row>
@@ -10815,23 +10812,23 @@
         <v>2320</v>
       </c>
       <c r="I116" s="1">
-        <f>COUNTIF($C$7:$C$89,$H116)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J116" s="1">
-        <f>SUMIF($C$7:$C$89,$H116,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="K116" s="1">
-        <f>SUMIF($C$7:$C$89,$H116,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>1024</v>
       </c>
       <c r="L116" s="1">
-        <f>SUMIF($C$7:$C$89,$H116,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>8050000</v>
       </c>
       <c r="M116" s="3">
-        <f>J116/(K116+J116)*100</f>
+        <f t="shared" si="4"/>
         <v>3.3050047214353167</v>
       </c>
     </row>
@@ -10840,23 +10837,23 @@
         <v>2313</v>
       </c>
       <c r="I117" s="1">
-        <f>COUNTIF($C$7:$C$89,$H117)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J117" s="1">
-        <f>SUMIF($C$7:$C$89,$H117,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="K117" s="1">
-        <f>SUMIF($C$7:$C$89,$H117,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>201</v>
       </c>
       <c r="L117" s="1">
-        <f>SUMIF($C$7:$C$89,$H117,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>5750000</v>
       </c>
       <c r="M117" s="3">
-        <f>J117/(K117+J117)*100</f>
+        <f t="shared" si="4"/>
         <v>11.061946902654867</v>
       </c>
     </row>
@@ -10865,23 +10862,23 @@
         <v>2327</v>
       </c>
       <c r="I118" s="1">
-        <f>COUNTIF($C$7:$C$89,$H118)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J118" s="1">
-        <f>SUMIF($C$7:$C$89,$H118,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="K118" s="1">
-        <f>SUMIF($C$7:$C$89,$H118,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>676</v>
       </c>
       <c r="L118" s="1">
-        <f>SUMIF($C$7:$C$89,$H118,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>5520000</v>
       </c>
       <c r="M118" s="3">
-        <f>J118/(K118+J118)*100</f>
+        <f t="shared" si="4"/>
         <v>3.4285714285714288</v>
       </c>
     </row>
@@ -10890,23 +10887,23 @@
         <v>2328</v>
       </c>
       <c r="I119" s="1">
-        <f>COUNTIF($C$7:$C$89,$H119)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J119" s="1">
-        <f>SUMIF($C$7:$C$89,$H119,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="K119" s="1">
-        <f>SUMIF($C$7:$C$89,$H119,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>364</v>
       </c>
       <c r="L119" s="1">
-        <f>SUMIF($C$7:$C$89,$H119,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>3680000</v>
       </c>
       <c r="M119" s="3">
-        <f>J119/(K119+J119)*100</f>
+        <f t="shared" si="4"/>
         <v>4.2105263157894735</v>
       </c>
     </row>
@@ -10915,23 +10912,23 @@
         <v>2323</v>
       </c>
       <c r="I120" s="1">
-        <f>COUNTIF($C$7:$C$89,$H120)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J120" s="1">
-        <f>SUMIF($C$7:$C$89,$H120,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="K120" s="1">
-        <f>SUMIF($C$7:$C$89,$H120,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>985</v>
       </c>
       <c r="L120" s="1">
-        <f>SUMIF($C$7:$C$89,$H120,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>3220000</v>
       </c>
       <c r="M120" s="3">
-        <f>J120/(K120+J120)*100</f>
+        <f t="shared" si="4"/>
         <v>1.4014014014014013</v>
       </c>
     </row>
@@ -10940,23 +10937,23 @@
         <v>2316</v>
       </c>
       <c r="I121" s="1">
-        <f>COUNTIF($C$7:$C$89,$H121)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J121" s="1">
-        <f>SUMIF($C$7:$C$89,$H121,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="K121" s="1">
-        <f>SUMIF($C$7:$C$89,$H121,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>609</v>
       </c>
       <c r="L121" s="1">
-        <f>SUMIF($C$7:$C$89,$H121,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>2990000</v>
       </c>
       <c r="M121" s="3">
-        <f>J121/(K121+J121)*100</f>
+        <f t="shared" si="4"/>
         <v>2.090032154340836</v>
       </c>
     </row>
@@ -10965,23 +10962,23 @@
         <v>2321</v>
       </c>
       <c r="I122" s="1">
-        <f>COUNTIF($C$7:$C$89,$H122)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J122" s="1">
-        <f>SUMIF($C$7:$C$89,$H122,D$7:D$89)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K122" s="1">
-        <f>SUMIF($C$7:$C$89,$H122,E$7:E$89)</f>
+        <f t="shared" si="2"/>
         <v>195</v>
       </c>
       <c r="L122" s="1">
-        <f>SUMIF($C$7:$C$89,$H122,F$7:F$89)</f>
+        <f t="shared" si="3"/>
         <v>230000</v>
       </c>
       <c r="M122" s="3">
-        <f>J122/(K122+J122)*100</f>
+        <f t="shared" si="4"/>
         <v>0.51020408163265307</v>
       </c>
     </row>

</xml_diff>